<commit_message>
Extra template files completed
</commit_message>
<xml_diff>
--- a/data/raw/Edubot_29 March 2024_10.43.xlsx
+++ b/data/raw/Edubot_29 March 2024_10.43.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CSBLR\Downloads\Edubot_29+March+2024_10.43\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gla-my.sharepoint.com/personal/2469113f_student_gla_ac_uk/Documents/Year 4/Dissertation/daniel-f-dissertation/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A141A4E2-4330-4C8C-90DB-13D7AB4FAB9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{A141A4E2-4330-4C8C-90DB-13D7AB4FAB9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A2F2E70-8B1D-4CBB-9F38-2DE8A159652B}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="247">
   <si>
     <t>StartDate</t>
   </si>
@@ -779,27 +779,6 @@
   </si>
   <si>
     <t xml:space="preserve"> If that is strong problem, the solution is to train lecturers better or remove them for something else, not to add an intermediary layer</t>
-  </si>
-  <si>
-    <t>Edubot - Human</t>
-  </si>
-  <si>
-    <t>Kineto - Human</t>
-  </si>
-  <si>
-    <t>AI Concept Generator  - MetaGPT</t>
-  </si>
-  <si>
-    <t>AI Tutor Mode - MetaGPT</t>
-  </si>
-  <si>
-    <t>Untitled 1  - Human</t>
-  </si>
-  <si>
-    <t>Edubot Explorer - ChatGPT</t>
-  </si>
-  <si>
-    <t>Communicaton  Simplification Bot - Human</t>
   </si>
 </sst>
 </file>
@@ -856,7 +835,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1196,7 +1175,7 @@
   <dimension ref="A1:FZ5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="AC8" sqref="AC8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2845,201 +2824,14 @@
         <v>246</v>
       </c>
     </row>
-    <row r="4" spans="1:182" x14ac:dyDescent="0.3">
-      <c r="AA4">
-        <f>GEOMEAN(V3:AA3)</f>
-        <v>2.3299861015014258</v>
-      </c>
-      <c r="AD4">
-        <f>GEOMEAN(AB3:AD3)</f>
-        <v>2</v>
-      </c>
-      <c r="AG4">
-        <f>GEOMEAN(AE3:AG3)</f>
-        <v>2</v>
-      </c>
-      <c r="AK4">
-        <f>GEOMEAN(AH3:AK3)</f>
-        <v>2.6321480259049852</v>
-      </c>
-      <c r="AO4">
-        <f>GEOMEAN(AL3:AO3)</f>
-        <v>2.5900200641113513</v>
-      </c>
-      <c r="AX4">
-        <f>GEOMEAN(AS3:AX3)</f>
-        <v>6.7439791373953524</v>
-      </c>
-      <c r="BA4">
-        <f>GEOMEAN(AY3:BA3)</f>
-        <v>3.6342411856642793</v>
-      </c>
-      <c r="BD4">
-        <f>GEOMEAN(BB3:BD3)</f>
-        <v>3.556893304490063</v>
-      </c>
-      <c r="BH4">
-        <f>GEOMEAN(BE3:BH3)</f>
-        <v>2.0597671439071177</v>
-      </c>
-      <c r="BL4">
-        <f>GEOMEAN(BI3:BL3)</f>
-        <v>3.0274001040350913</v>
-      </c>
-      <c r="BU4">
-        <f>GEOMEAN(BP3:BU3)</f>
-        <v>4.6415888336127793</v>
-      </c>
-      <c r="BX4">
-        <f>GEOMEAN(BV3:BX3)</f>
-        <v>4.6415888336127793</v>
-      </c>
-      <c r="CA4">
-        <f>GEOMEAN(BY3:CA3)</f>
-        <v>4</v>
-      </c>
-      <c r="CE4">
-        <f>GEOMEAN(CB3:CE3)</f>
-        <v>4.1195342878142354</v>
-      </c>
-      <c r="CI4">
-        <f>GEOMEAN(CF3:CI3)</f>
-        <v>3.9359793425308607</v>
-      </c>
-      <c r="CR4">
-        <f>GEOMEAN(CM3:CR3)</f>
-        <v>2.3299861015014258</v>
-      </c>
-      <c r="CU4">
-        <f>GEOMEAN(CS3:CU3)</f>
-        <v>2.6207413942088964</v>
-      </c>
-      <c r="CX4">
-        <f>GEOMEAN(CV3:CX3)</f>
-        <v>1.5874010519681994</v>
-      </c>
-      <c r="DB4">
-        <f>GEOMEAN(CY3:DB3)</f>
-        <v>3.7224194364083982</v>
-      </c>
-      <c r="DF4">
-        <f>GEOMEAN(DC3:DF3)</f>
-        <v>2.0597671439071177</v>
-      </c>
-      <c r="DO4">
-        <f>GEOMEAN(DJ3:DO3)</f>
-        <v>7.05093753307046</v>
-      </c>
-      <c r="DR4">
-        <f>GEOMEAN(DP3:DR3)</f>
-        <v>7.6517247310895558</v>
-      </c>
-      <c r="DU4">
-        <f>GEOMEAN(DS3:DU3)</f>
-        <v>7.6517247310895558</v>
-      </c>
-      <c r="DY4">
-        <f>GEOMEAN(DV3:DY3)</f>
-        <v>7.4833147735478827</v>
-      </c>
-      <c r="EC4">
-        <f>GEOMEAN(DZ3:EC3)</f>
-        <v>6.9640090904541871</v>
-      </c>
-      <c r="EG4">
-        <v>3</v>
-      </c>
-      <c r="EL4">
-        <f>GEOMEAN(EG3:EL3)</f>
-        <v>4.9660971338974731</v>
-      </c>
-      <c r="EO4">
-        <f>GEOMEAN(EM3:EO3)</f>
-        <v>4.6415888336127793</v>
-      </c>
-      <c r="ER4">
-        <f>GEOMEAN(EP3:ER3)</f>
-        <v>4</v>
-      </c>
-      <c r="EV4">
-        <f>GEOMEAN(ES3:EV3)</f>
-        <v>4.6806946386414321</v>
-      </c>
-      <c r="EZ4">
-        <f>GEOMEAN(EW3:EZ3)</f>
-        <v>4.2294850537622564</v>
-      </c>
-      <c r="FI4">
-        <f>GEOMEAN(FD3:FI3)</f>
-        <v>3.9572048929358528</v>
-      </c>
-      <c r="FL4">
-        <f>GEOMEAN(FJ3:FL3)</f>
-        <v>4.5788569702133275</v>
-      </c>
-      <c r="FO4">
-        <f>GEOMEAN(FM3:FO3)</f>
-        <v>2.8844991406148166</v>
-      </c>
-      <c r="FS4">
-        <f>GEOMEAN(FP3:FS3)</f>
-        <v>3.1301691601465746</v>
-      </c>
-      <c r="FW4">
-        <f>GEOMEAN(FT3:FW3)</f>
-        <v>2.6321480259049852</v>
-      </c>
-    </row>
     <row r="5" spans="1:182" x14ac:dyDescent="0.3">
-      <c r="V5" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="AO5">
-        <f>SUM(AA4:AO4)</f>
-        <v>11.552154191517763</v>
-      </c>
-      <c r="AS5" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="BL5">
-        <f>SUM(AX4:BL4)</f>
-        <v>19.022280875491901</v>
-      </c>
-      <c r="BP5" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="CI5">
-        <f>SUM(BU4:CI4)</f>
-        <v>21.338691297570655</v>
-      </c>
-      <c r="CM5" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="DF5">
-        <f>SUM(CR4:DF4)</f>
-        <v>12.320315127994037</v>
-      </c>
-      <c r="DJ5" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="EC5">
-        <f>SUM(DO4:EC4)</f>
-        <v>36.801710859251642</v>
-      </c>
-      <c r="EG5" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="EZ5">
-        <f>SUM(EL4:EZ4)</f>
-        <v>22.517865659913941</v>
-      </c>
-      <c r="FD5" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="FW5">
-        <f>SUM(FI4:FW4)</f>
-        <v>17.182878189815558</v>
-      </c>
+      <c r="V5" s="4"/>
+      <c r="AS5" s="4"/>
+      <c r="BP5" s="4"/>
+      <c r="CM5" s="4"/>
+      <c r="DJ5" s="4"/>
+      <c r="EG5" s="4"/>
+      <c r="FD5" s="4"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:FZ4" xr:uid="{00000000-0009-0000-0000-000000000000}"/>

</xml_diff>